<commit_message>
Monte Carlo Type AI
The AI now simulates 1000 games with random moves to decide which move
to use. The first move is always recorded and if the game is won then
that is tallied up. The move that won the most random games is the move
that is chosen.
</commit_message>
<xml_diff>
--- a/Enemy1.xlsx
+++ b/Enemy1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="4460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -647,10 +647,10 @@
         <v>200</v>
       </c>
       <c r="H2">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="I2">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="J2">
         <v>90</v>
@@ -739,10 +739,10 @@
         <v>70000</v>
       </c>
       <c r="H3">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="I3">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="J3">
         <v>50</v>

</xml_diff>